<commit_message>
Add comparison for large instances
</commit_message>
<xml_diff>
--- a/comparison_IPA_default.xlsx
+++ b/comparison_IPA_default.xlsx
@@ -8,13 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://sotonac-my.sharepoint.com/personal/mj1v21_soton_ac_uk/Documents/Hyperplane_clustering/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="180" documentId="8_{DE50E83A-DD7F-42E6-8645-5AABE850345B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AA845A35-B765-4805-A1AB-09EC4D6A7AB6}"/>
+  <xr:revisionPtr revIDLastSave="429" documentId="8_{DE50E83A-DD7F-42E6-8645-5AABE850345B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{60DE89FF-7D5A-4859-B40C-30D172485ABC}"/>
   <bookViews>
-    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{B6873EE8-1297-46A4-A3F6-D9DB06214473}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{B6873EE8-1297-46A4-A3F6-D9DB06214473}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="30">
   <si>
     <t>#dimensions</t>
   </si>
@@ -88,6 +90,45 @@
   </si>
   <si>
     <t>IPA time</t>
+  </si>
+  <si>
+    <t>Ratio</t>
+  </si>
+  <si>
+    <t>tol</t>
+  </si>
+  <si>
+    <t>10^-8, 10^-4</t>
+  </si>
+  <si>
+    <t>10^-3</t>
+  </si>
+  <si>
+    <t>10^-2</t>
+  </si>
+  <si>
+    <t>Out of memory</t>
+  </si>
+  <si>
+    <t>License limitation</t>
+  </si>
+  <si>
+    <t>IPA swap label</t>
+  </si>
+  <si>
+    <t>Bound of level 1</t>
+  </si>
+  <si>
+    <t>OG</t>
+  </si>
+  <si>
+    <t>Swap label</t>
+  </si>
+  <si>
+    <t>IPA with 10% projected sol</t>
+  </si>
+  <si>
+    <t>IPA with 10% projected sol + swap label</t>
   </si>
 </sst>
 </file>
@@ -123,8 +164,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -453,8 +497,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{47F1A8AB-03E0-47C3-8289-F2AA35A1D3FB}">
   <dimension ref="A1:J17"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+    <sheetView zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -464,28 +508,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4" t="s">
+      <c r="D1" s="5"/>
+      <c r="E1" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4" t="s">
+      <c r="F1" s="5"/>
+      <c r="G1" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="4"/>
+      <c r="H1" s="5"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="4"/>
-      <c r="B2" s="4"/>
+      <c r="A2" s="5"/>
+      <c r="B2" s="5"/>
       <c r="C2" s="1" t="s">
         <v>3</v>
       </c>
@@ -948,42 +992,47 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C46BA01F-D704-4F87-BFAE-6992AED85787}">
-  <dimension ref="A1:I16"/>
+  <dimension ref="A1:O16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L17" sqref="L17"/>
+    <sheetView zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection sqref="A1:J16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.5703125" customWidth="1"/>
-    <col min="8" max="8" width="7.85546875" customWidth="1"/>
+    <col min="8" max="8" width="7.85546875" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="13" customWidth="1"/>
+    <col min="13" max="13" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4" t="s">
+      <c r="D1" s="5"/>
+      <c r="E1" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4" t="s">
+      <c r="F1" s="5"/>
+      <c r="G1" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="4"/>
-      <c r="I1" s="4"/>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="4"/>
-      <c r="B2" s="4"/>
+      <c r="H1" s="5"/>
+      <c r="I1" s="5"/>
+      <c r="J1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A2" s="5"/>
+      <c r="B2" s="5"/>
       <c r="C2" s="3" t="s">
         <v>3</v>
       </c>
@@ -1006,7 +1055,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>3</v>
       </c>
@@ -1035,8 +1084,12 @@
         <f>H3-D3</f>
         <v>0.31</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J3">
+        <f>I3/D3</f>
+        <v>1.7222222222222223</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1065,8 +1118,24 @@
         <f t="shared" ref="I4:I16" si="0">H4-D4</f>
         <v>0.19999999999999998</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J4">
+        <f t="shared" ref="J4:J16" si="1">I4/D4</f>
+        <v>1.3333333333333333</v>
+      </c>
+      <c r="L4" t="s">
+        <v>18</v>
+      </c>
+      <c r="M4" t="s">
+        <v>19</v>
+      </c>
+      <c r="N4" t="s">
+        <v>20</v>
+      </c>
+      <c r="O4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>3</v>
       </c>
@@ -1095,8 +1164,24 @@
         <f t="shared" si="0"/>
         <v>0.49000000000000005</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J5">
+        <f t="shared" si="1"/>
+        <v>1.6896551724137934</v>
+      </c>
+      <c r="L5" t="s">
+        <v>3</v>
+      </c>
+      <c r="M5">
+        <v>320</v>
+      </c>
+      <c r="N5">
+        <v>312</v>
+      </c>
+      <c r="O5">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>3</v>
       </c>
@@ -1125,8 +1210,12 @@
         <f t="shared" si="0"/>
         <v>0.32</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J6">
+        <f t="shared" si="1"/>
+        <v>1.1034482758620692</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>3</v>
       </c>
@@ -1155,8 +1244,12 @@
         <f t="shared" si="0"/>
         <v>0.47</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J7">
+        <f t="shared" si="1"/>
+        <v>1.2368421052631577</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>3</v>
       </c>
@@ -1185,8 +1278,12 @@
         <f t="shared" si="0"/>
         <v>0.48</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J8">
+        <f t="shared" si="1"/>
+        <v>0.92307692307692302</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>4</v>
       </c>
@@ -1215,8 +1312,12 @@
         <f t="shared" si="0"/>
         <v>0.45999999999999996</v>
       </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J9">
+        <f t="shared" si="1"/>
+        <v>2.7058823529411762</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>4</v>
       </c>
@@ -1245,8 +1346,12 @@
         <f t="shared" si="0"/>
         <v>0.57999999999999996</v>
       </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J10">
+        <f t="shared" si="1"/>
+        <v>3.4117647058823524</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>4</v>
       </c>
@@ -1275,8 +1380,12 @@
         <f t="shared" si="0"/>
         <v>1.1599999999999999</v>
       </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J11">
+        <f t="shared" si="1"/>
+        <v>3.7419354838709675</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>4</v>
       </c>
@@ -1305,8 +1414,12 @@
         <f t="shared" si="0"/>
         <v>3.16</v>
       </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J12">
+        <f t="shared" si="1"/>
+        <v>7.5238095238095246</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>5</v>
       </c>
@@ -1335,8 +1448,12 @@
         <f t="shared" si="0"/>
         <v>1.1300000000000001</v>
       </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J13">
+        <f t="shared" si="1"/>
+        <v>5.9473684210526319</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>5</v>
       </c>
@@ -1365,8 +1482,12 @@
         <f t="shared" si="0"/>
         <v>0.52</v>
       </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J14">
+        <f t="shared" si="1"/>
+        <v>4.7272727272727275</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>5</v>
       </c>
@@ -1395,8 +1516,12 @@
         <f t="shared" si="0"/>
         <v>1.4300000000000002</v>
       </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J15">
+        <f t="shared" si="1"/>
+        <v>8.9375</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>5</v>
       </c>
@@ -1424,6 +1549,10 @@
       <c r="I16">
         <f t="shared" si="0"/>
         <v>6.79</v>
+      </c>
+      <c r="J16">
+        <f t="shared" si="1"/>
+        <v>22.633333333333333</v>
       </c>
     </row>
   </sheetData>
@@ -1437,4 +1566,725 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{82ABE362-62FA-415B-B700-B016F664780C}">
+  <dimension ref="A1:V15"/>
+  <sheetViews>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="V20" sqref="V20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="16" max="16" width="14.140625" customWidth="1"/>
+    <col min="19" max="19" width="17.42578125" customWidth="1"/>
+    <col min="22" max="22" width="27.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="5"/>
+      <c r="I1" s="5"/>
+      <c r="J1" t="s">
+        <v>17</v>
+      </c>
+      <c r="L1" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="M1" s="5"/>
+      <c r="O1" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="P1" s="5"/>
+      <c r="R1" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="S1" s="5"/>
+      <c r="U1" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="V1" s="5"/>
+    </row>
+    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A2" s="5"/>
+      <c r="B2" s="5"/>
+      <c r="C2" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="L2" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="M2" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="O2" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="P2" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="R2" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="S2" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="U2" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="V2" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>500</v>
+      </c>
+      <c r="C3">
+        <v>20</v>
+      </c>
+      <c r="D3">
+        <v>0.7</v>
+      </c>
+      <c r="E3">
+        <v>42</v>
+      </c>
+      <c r="F3">
+        <v>0.17</v>
+      </c>
+      <c r="G3">
+        <v>24</v>
+      </c>
+      <c r="H3">
+        <v>0.86</v>
+      </c>
+      <c r="I3">
+        <f>H3-D3</f>
+        <v>0.16000000000000003</v>
+      </c>
+      <c r="J3">
+        <f>I3/D3</f>
+        <v>0.22857142857142862</v>
+      </c>
+      <c r="L3">
+        <v>60.887300000000003</v>
+      </c>
+      <c r="M3">
+        <v>60.481699999999996</v>
+      </c>
+      <c r="O3">
+        <v>38</v>
+      </c>
+      <c r="P3">
+        <v>0.16</v>
+      </c>
+      <c r="R3">
+        <v>42</v>
+      </c>
+      <c r="S3">
+        <v>0.13</v>
+      </c>
+      <c r="U3">
+        <v>40</v>
+      </c>
+      <c r="V3">
+        <v>0.17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <v>1000</v>
+      </c>
+      <c r="C4">
+        <v>33</v>
+      </c>
+      <c r="D4">
+        <v>1.77</v>
+      </c>
+      <c r="E4">
+        <v>45</v>
+      </c>
+      <c r="F4">
+        <v>0.21</v>
+      </c>
+      <c r="G4">
+        <v>28</v>
+      </c>
+      <c r="H4">
+        <v>1.97</v>
+      </c>
+      <c r="I4">
+        <f t="shared" ref="I4:I14" si="0">H4-D4</f>
+        <v>0.19999999999999996</v>
+      </c>
+      <c r="J4">
+        <f t="shared" ref="J4:J14" si="1">I4/D4</f>
+        <v>0.11299435028248585</v>
+      </c>
+      <c r="L4">
+        <v>118.188</v>
+      </c>
+      <c r="M4">
+        <v>121.38800000000001</v>
+      </c>
+      <c r="O4">
+        <v>45</v>
+      </c>
+      <c r="P4">
+        <v>0.24</v>
+      </c>
+      <c r="R4">
+        <v>38</v>
+      </c>
+      <c r="S4">
+        <v>0.16</v>
+      </c>
+      <c r="U4">
+        <v>38</v>
+      </c>
+      <c r="V4">
+        <v>0.22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>2</v>
+      </c>
+      <c r="B5">
+        <v>1500</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D5" s="5"/>
+      <c r="E5">
+        <v>42</v>
+      </c>
+      <c r="F5">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="L5">
+        <v>182.458</v>
+      </c>
+      <c r="M5">
+        <v>184.39</v>
+      </c>
+      <c r="O5">
+        <v>38</v>
+      </c>
+      <c r="P5">
+        <v>0.35</v>
+      </c>
+      <c r="R5">
+        <v>38</v>
+      </c>
+      <c r="S5">
+        <v>0.24</v>
+      </c>
+      <c r="U5">
+        <v>38</v>
+      </c>
+      <c r="V5">
+        <v>0.27</v>
+      </c>
+    </row>
+    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>2</v>
+      </c>
+      <c r="B6">
+        <v>2000</v>
+      </c>
+      <c r="E6">
+        <v>43</v>
+      </c>
+      <c r="F6">
+        <v>0.33</v>
+      </c>
+      <c r="L6">
+        <v>246.41800000000001</v>
+      </c>
+      <c r="M6">
+        <v>242.584</v>
+      </c>
+      <c r="O6">
+        <v>44</v>
+      </c>
+      <c r="P6">
+        <v>0.42</v>
+      </c>
+      <c r="R6">
+        <v>34</v>
+      </c>
+      <c r="S6">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="U6">
+        <v>34</v>
+      </c>
+      <c r="V6">
+        <v>0.38</v>
+      </c>
+    </row>
+    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>2</v>
+      </c>
+      <c r="B7">
+        <v>2500</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="F7" s="5"/>
+      <c r="O7" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="P7" s="5"/>
+    </row>
+    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>3</v>
+      </c>
+      <c r="B8">
+        <v>500</v>
+      </c>
+      <c r="C8">
+        <v>629</v>
+      </c>
+      <c r="D8">
+        <v>1.0900000000000001</v>
+      </c>
+      <c r="E8">
+        <v>592</v>
+      </c>
+      <c r="F8">
+        <v>0.91</v>
+      </c>
+      <c r="G8">
+        <v>316</v>
+      </c>
+      <c r="H8">
+        <v>1.71</v>
+      </c>
+      <c r="I8">
+        <f t="shared" si="0"/>
+        <v>0.61999999999999988</v>
+      </c>
+      <c r="J8">
+        <f t="shared" si="1"/>
+        <v>0.56880733944954109</v>
+      </c>
+      <c r="L8">
+        <v>61.055799999999998</v>
+      </c>
+      <c r="M8">
+        <v>60.5319</v>
+      </c>
+      <c r="O8">
+        <v>367</v>
+      </c>
+      <c r="P8">
+        <v>0.87</v>
+      </c>
+      <c r="R8">
+        <v>551</v>
+      </c>
+      <c r="S8">
+        <v>0.87</v>
+      </c>
+      <c r="U8">
+        <v>437</v>
+      </c>
+      <c r="V8">
+        <v>0.86</v>
+      </c>
+    </row>
+    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>3</v>
+      </c>
+      <c r="B9">
+        <v>1000</v>
+      </c>
+      <c r="C9">
+        <v>754</v>
+      </c>
+      <c r="D9">
+        <v>2.4700000000000002</v>
+      </c>
+      <c r="E9">
+        <v>536</v>
+      </c>
+      <c r="F9">
+        <v>1.27</v>
+      </c>
+      <c r="G9">
+        <v>254</v>
+      </c>
+      <c r="H9">
+        <v>3.09</v>
+      </c>
+      <c r="I9">
+        <f t="shared" si="0"/>
+        <v>0.61999999999999966</v>
+      </c>
+      <c r="J9">
+        <f t="shared" si="1"/>
+        <v>0.25101214574898773</v>
+      </c>
+      <c r="L9">
+        <v>119.536</v>
+      </c>
+      <c r="M9">
+        <v>116.547</v>
+      </c>
+      <c r="O9">
+        <v>377</v>
+      </c>
+      <c r="P9">
+        <v>1.1499999999999999</v>
+      </c>
+      <c r="R9">
+        <v>541</v>
+      </c>
+      <c r="S9">
+        <v>1.23</v>
+      </c>
+      <c r="U9">
+        <v>437</v>
+      </c>
+      <c r="V9">
+        <v>1.44</v>
+      </c>
+    </row>
+    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>3</v>
+      </c>
+      <c r="B10">
+        <v>1500</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D10" s="5"/>
+      <c r="E10">
+        <v>467</v>
+      </c>
+      <c r="F10">
+        <v>1.42</v>
+      </c>
+      <c r="L10">
+        <v>184.91499999999999</v>
+      </c>
+      <c r="M10">
+        <v>172.83099999999999</v>
+      </c>
+      <c r="O10">
+        <v>422</v>
+      </c>
+      <c r="P10">
+        <v>1.7</v>
+      </c>
+      <c r="R10">
+        <v>686</v>
+      </c>
+      <c r="S10">
+        <v>2.0299999999999998</v>
+      </c>
+      <c r="U10">
+        <v>506</v>
+      </c>
+      <c r="V10">
+        <v>1.92</v>
+      </c>
+    </row>
+    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>3</v>
+      </c>
+      <c r="B11">
+        <v>2000</v>
+      </c>
+      <c r="E11">
+        <v>556</v>
+      </c>
+      <c r="F11">
+        <v>2.13</v>
+      </c>
+      <c r="L11">
+        <v>246.90899999999999</v>
+      </c>
+      <c r="M11">
+        <v>231.964</v>
+      </c>
+      <c r="O11">
+        <v>436</v>
+      </c>
+      <c r="P11">
+        <v>2.0299999999999998</v>
+      </c>
+      <c r="R11">
+        <v>455</v>
+      </c>
+      <c r="S11">
+        <v>1.78</v>
+      </c>
+      <c r="U11">
+        <v>419</v>
+      </c>
+      <c r="V11">
+        <v>1.98</v>
+      </c>
+    </row>
+    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>3</v>
+      </c>
+      <c r="B12">
+        <v>2500</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="F12" s="5"/>
+      <c r="O12" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="P12" s="5"/>
+    </row>
+    <row r="13" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>4</v>
+      </c>
+      <c r="B13">
+        <v>500</v>
+      </c>
+      <c r="C13">
+        <v>127</v>
+      </c>
+      <c r="D13">
+        <v>0.91</v>
+      </c>
+      <c r="E13">
+        <v>1854</v>
+      </c>
+      <c r="F13">
+        <v>2.4900000000000002</v>
+      </c>
+      <c r="G13">
+        <v>1450</v>
+      </c>
+      <c r="H13">
+        <v>3.06</v>
+      </c>
+      <c r="I13">
+        <f t="shared" si="0"/>
+        <v>2.15</v>
+      </c>
+      <c r="J13">
+        <f t="shared" si="1"/>
+        <v>2.3626373626373622</v>
+      </c>
+      <c r="L13">
+        <v>53.677999999999997</v>
+      </c>
+      <c r="M13">
+        <v>56.575000000000003</v>
+      </c>
+      <c r="O13">
+        <v>1858</v>
+      </c>
+      <c r="P13">
+        <v>3.59</v>
+      </c>
+      <c r="R13">
+        <v>3998</v>
+      </c>
+      <c r="S13">
+        <v>5.52</v>
+      </c>
+      <c r="U13">
+        <v>3666</v>
+      </c>
+      <c r="V13">
+        <v>6.83</v>
+      </c>
+    </row>
+    <row r="14" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>4</v>
+      </c>
+      <c r="B14">
+        <v>1000</v>
+      </c>
+      <c r="C14">
+        <v>550</v>
+      </c>
+      <c r="D14">
+        <v>2.84</v>
+      </c>
+      <c r="E14">
+        <v>5430</v>
+      </c>
+      <c r="F14">
+        <v>9.83</v>
+      </c>
+      <c r="G14">
+        <v>4346</v>
+      </c>
+      <c r="H14">
+        <v>10.78</v>
+      </c>
+      <c r="I14">
+        <f t="shared" si="0"/>
+        <v>7.9399999999999995</v>
+      </c>
+      <c r="J14">
+        <f t="shared" si="1"/>
+        <v>2.795774647887324</v>
+      </c>
+      <c r="L14">
+        <v>118.797</v>
+      </c>
+      <c r="M14">
+        <v>117.185</v>
+      </c>
+      <c r="O14">
+        <v>5230</v>
+      </c>
+      <c r="P14">
+        <v>12.85</v>
+      </c>
+      <c r="R14">
+        <v>26250</v>
+      </c>
+      <c r="S14">
+        <v>45.95</v>
+      </c>
+      <c r="U14">
+        <v>24678</v>
+      </c>
+      <c r="V14">
+        <v>58.49</v>
+      </c>
+    </row>
+    <row r="15" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>4</v>
+      </c>
+      <c r="B15">
+        <v>1500</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D15" s="5"/>
+      <c r="E15">
+        <v>7230</v>
+      </c>
+      <c r="F15">
+        <v>18</v>
+      </c>
+      <c r="L15">
+        <v>186.38800000000001</v>
+      </c>
+      <c r="M15">
+        <v>173.12100000000001</v>
+      </c>
+      <c r="O15">
+        <v>7114</v>
+      </c>
+      <c r="P15">
+        <v>23.8</v>
+      </c>
+      <c r="R15">
+        <v>17784</v>
+      </c>
+      <c r="S15">
+        <v>47.83</v>
+      </c>
+      <c r="U15">
+        <v>17314</v>
+      </c>
+      <c r="V15">
+        <v>53.68</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="16">
+    <mergeCell ref="O1:P1"/>
+    <mergeCell ref="O7:P7"/>
+    <mergeCell ref="O12:P12"/>
+    <mergeCell ref="U1:V1"/>
+    <mergeCell ref="R1:S1"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="C10:D10"/>
+    <mergeCell ref="E12:F12"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="L1:M1"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="E1:F1"/>
+    <mergeCell ref="G1:I1"/>
+    <mergeCell ref="C5:D5"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{02B98E8C-6886-4249-BC4B-E89D5CF9DEB2}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>